<commit_message>
Latest one with Jenkins Integration!!!
</commit_message>
<xml_diff>
--- a/resources/Test_Runner.xlsx
+++ b/resources/Test_Runner.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\450405\.jenkins\workspace\TestAutomation\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="19155" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="19155" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="TestRunner" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
   <si>
     <t>S.No</t>
   </si>
@@ -42,9 +47,6 @@
     <t>App_type</t>
   </si>
   <si>
-    <t>Windows</t>
-  </si>
-  <si>
     <t>NotApplicable</t>
   </si>
   <si>
@@ -87,18 +89,6 @@
     <t>Local</t>
   </si>
   <si>
-    <t>Google Chrome</t>
-  </si>
-  <si>
-    <t>Firefox</t>
-  </si>
-  <si>
-    <t>http://www.bing.com</t>
-  </si>
-  <si>
-    <t>API_Test</t>
-  </si>
-  <si>
     <t>Endpoint</t>
   </si>
   <si>
@@ -138,89 +128,119 @@
     <t>https://dt.pulsenow.co.uk</t>
   </si>
   <si>
-    <t>Do Post request with parameters</t>
-  </si>
-  <si>
     <t>https://regno.pulsenow.co.uk</t>
   </si>
   <si>
     <t>/mobile/customerinfo/v2/postcode/DM001PL</t>
   </si>
   <si>
-    <t>Do Get request with headers</t>
-  </si>
-  <si>
-    <t>Do Get request without headers and parameters</t>
-  </si>
-  <si>
     <t>Run</t>
   </si>
   <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Header_1:</t>
+  </si>
+  <si>
+    <t>Header_2</t>
+  </si>
+  <si>
+    <t>URLParam_1:id</t>
+  </si>
+  <si>
+    <t>saced</t>
+  </si>
+  <si>
+    <t>Json_File_Name</t>
+  </si>
+  <si>
+    <t>http://debcomtst1.directenergy.com/small-business/products?appSourceCode=ORMXN</t>
+  </si>
+  <si>
+    <t>BaseURL</t>
+  </si>
+  <si>
+    <t>Organic flow for small businesses</t>
+  </si>
+  <si>
+    <t>07001</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>a@a.com</t>
+  </si>
+  <si>
+    <t>8708098090</t>
+  </si>
+  <si>
+    <t>Street Name</t>
+  </si>
+  <si>
+    <t>0003</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>VISTA</t>
+  </si>
+  <si>
+    <t>60001</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Functional</t>
-  </si>
-  <si>
-    <t>Search a text 'Firefox' in Bing</t>
-  </si>
-  <si>
-    <t>Header_1:</t>
-  </si>
-  <si>
-    <t>Google</t>
+    <t>Headless</t>
+  </si>
+  <si>
+    <t>http://the-internet.herokuapp.com/broken_images</t>
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>http://localhost:8080</t>
-  </si>
-  <si>
-    <t>Header_2</t>
-  </si>
-  <si>
-    <t>URLParam_1:id</t>
-  </si>
-  <si>
-    <t>saced</t>
-  </si>
-  <si>
-    <t>/dali/api/ephemeral/field/services/jobs/update</t>
-  </si>
-  <si>
-    <t>Json_File_Name</t>
-  </si>
-  <si>
-    <t>sachin</t>
-  </si>
-  <si>
-    <t>GET Salvador</t>
-  </si>
-  <si>
-    <t>PUT Salvador</t>
-  </si>
-  <si>
-    <t>DELETE Salvador</t>
-  </si>
-  <si>
-    <t>When I open Google website;And I enter some text;Then I should see that text in the result page</t>
-  </si>
-  <si>
-    <t>UPDATE Salvador</t>
-  </si>
-  <si>
-    <t>sachin-update</t>
-  </si>
-  <si>
-    <t>salvador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,10 +294,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -285,6 +306,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -331,7 +360,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -363,9 +392,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -397,6 +427,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -572,14 +603,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="88" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" customWidth="1"/>
@@ -590,7 +621,7 @@
     <col min="9" max="9" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -604,7 +635,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -616,10 +647,10 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -627,28 +658,28 @@
         <v>1001</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
       <c r="I2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -656,249 +687,46 @@
         <v>1002</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
       <c r="I3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1003</v>
-      </c>
-      <c r="C4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1004</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1005</v>
-      </c>
-      <c r="C6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>1006</v>
-      </c>
-      <c r="C7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>1007</v>
-      </c>
-      <c r="C8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>1008</v>
-      </c>
-      <c r="C9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>1009</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
       <formula1>"Functional,UX_Test,API_Test,Load_Test,Performance_Test"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F10">
-      <formula1>"Windows,Mac,Android,iOS"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G10">
-      <formula1>"Google Chrome,Firefox,IE,Edge,Safari,NotApplicable"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3">
       <formula1>"Native,Hybrid,WebApp,NotApplicable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I3">
       <formula1>"Local,Remote"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3">
       <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3">
+      <formula1>"Windows,VISTA,Mac,Android,iOS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3">
+      <formula1>"Google Chrome,Firefox,IE,Edge,Safari,Headless,NotApplicable"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -906,21 +734,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -928,34 +759,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>54</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -963,13 +797,37 @@
         <v>1001</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>68</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -977,58 +835,40 @@
         <v>1002</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1003</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1004</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1005</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
@@ -1036,20 +876,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1057,34 +897,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1092,10 +932,10 @@
         <v>1002</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1107,16 +947,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.85546875" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" bestFit="1" customWidth="1"/>
@@ -1128,7 +968,7 @@
     <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1136,37 +976,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1174,13 +1014,13 @@
         <v>1001</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1188,28 +1028,28 @@
         <v>1002</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" t="s">
-        <v>34</v>
-      </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="L3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1217,119 +1057,122 @@
         <v>1003</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>1006</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>1007</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" t="s">
-        <v>57</v>
-      </c>
-      <c r="L6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>1008</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" t="s">
-        <v>63</v>
-      </c>
-      <c r="L7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>1009</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" t="s">
-        <v>64</v>
-      </c>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C8" r:id="rId6"/>
-    <hyperlink ref="C7" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1337,34 +1180,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1372,10 +1215,10 @@
         <v>1004</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1387,20 +1230,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1408,34 +1251,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1443,10 +1286,16 @@
         <v>1005</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
+      <c r="E2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>